<commit_message>
On branch master  Your branch is up to date with 'origin/master'.
 Changes to be committed:
	modified:   .Rhistory
	new file:   code/ATAC_04.Rmd
	new file:   code/ATAC_04.html
	new file:   code/ATAC_05.Rmd
	new file:   code/ATAC_05.html
	modified:   data/.DS_Store
	modified:   data/metadata.xlsx
	new file:   results/figures/ATAC_01_commonNFR.png
	new file:   results/figures/ATAC_02_NFRupset.png
	new file:   results/figures/ATAC_S01_NFRbarplot.png
	new file:   results/tables/ATAC_SupplementaryTable_01.xlsx
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityhealthnetwork-my.sharepoint.com/personal/emma_bell_uhnresearch_ca/Documents/Projects/02_Submitted/2020_LooBell_NatureMedicine/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98618F51-CB75-094E-AAF5-AD73ED78382D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{98618F51-CB75-094E-AAF5-AD73ED78382D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FF51981-9AD0-7149-8584-EF1A527E7559}"/>
   <bookViews>
-    <workbookView xWindow="37660" yWindow="2260" windowWidth="27640" windowHeight="16940" xr2:uid="{8098B32F-899C-864D-A40B-B974A9C6386F}"/>
+    <workbookView xWindow="3180" yWindow="1020" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{8098B32F-899C-864D-A40B-B974A9C6386F}"/>
   </bookViews>
   <sheets>
     <sheet name="RRBS" sheetId="1" r:id="rId1"/>
+    <sheet name="ATAC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>H1</t>
   </si>
@@ -93,6 +94,39 @@
   </si>
   <si>
     <t>Donor ID (simple)</t>
+  </si>
+  <si>
+    <t>Donor</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Donor61_stimulated_treated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor61_unstimulated_untreated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor61_stimulated_untreated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor70_unstimulated_untreated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor70_stimulated_untreated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor70_stimulated_treated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor71_unstimulated_untreated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor71_stimulated_untreated.narrowPeak</t>
+  </si>
+  <si>
+    <t>Donor71_stimulated_treated.narrowPeak</t>
   </si>
 </sst>
 </file>
@@ -161,6 +195,22 @@
     <tableColumn id="3" xr3:uid="{629416D1-C0E4-AC44-AC89-69FDEAF2A2E1}" name="Donor ID (simple)"/>
     <tableColumn id="4" xr3:uid="{E88885FF-08D3-F741-A747-0E2936742F6D}" name="Stimulated"/>
     <tableColumn id="5" xr3:uid="{0760876B-B9B3-F64B-8C7F-A0775045BD2A}" name="DAC"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{569738A9-CF51-264E-BAB2-557244D71843}" name="Table2" displayName="Table2" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10" xr:uid="{03B9F244-300A-8C43-82AF-36C383C4D9A3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D10">
+    <sortCondition ref="B1:B10"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{96BA2B96-B3CB-804D-8412-71FF4535E91F}" name="File"/>
+    <tableColumn id="2" xr3:uid="{9FD5BC55-6BF7-4E40-89BD-398268190BB4}" name="Donor"/>
+    <tableColumn id="3" xr3:uid="{4E0D881C-2B8B-C849-8199-C925DD9380EB}" name="Stimulated"/>
+    <tableColumn id="4" xr3:uid="{258361B5-7629-884F-95EE-E7C96922CDA9}" name="DAC"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -465,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A72CDEA-F026-7641-BB53-1C2C1D23D39F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -654,4 +704,166 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A69FB6-F2F2-1C4E-A6AD-2D5E1602C2C7}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>